<commit_message>
Edit the table of func
</commit_message>
<xml_diff>
--- a/Documents/Table of func.xlsx
+++ b/Documents/Table of func.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Карина\Desktop\HistoryProject-SherlockHomies\Documents\Q&amp;A doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Карина\Desktop\HistoryProject-SherlockHomies\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6484181-4E8C-45DB-B177-7FF0510E9931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BDAC7764-88BC-4717-8148-CB0825BFD10A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A0311DF7-80F3-4160-AC8A-0094427EBAF7}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Purpose</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>isEmpty()</t>
   </si>
   <si>
@@ -98,9 +95,6 @@
   </si>
   <si>
     <t>mainMenu()</t>
-  </si>
-  <si>
-    <t>Passed</t>
   </si>
   <si>
     <t>Insert the functions</t>
@@ -234,13 +228,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4FA18472-F8DB-457F-8C79-8B1B635EDF0D}" name="Table1" displayName="Table1" ref="A1:D15" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:D15" xr:uid="{4FA18472-F8DB-457F-8C79-8B1B635EDF0D}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4FA18472-F8DB-457F-8C79-8B1B635EDF0D}" name="Table1" displayName="Table1" ref="A1:C15" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:C15" xr:uid="{4FA18472-F8DB-457F-8C79-8B1B635EDF0D}"/>
+  <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{3E91630A-8497-4E54-AEAB-734A5D1D1D66}" name="Name"/>
     <tableColumn id="2" xr3:uid="{2D29D0D2-A9E7-495F-B0CE-1FF1CE261750}" name="Type"/>
     <tableColumn id="3" xr3:uid="{656A44CF-CD37-4A5D-ACAE-6545BEAEF7F0}" name="Purpose"/>
-    <tableColumn id="4" xr3:uid="{4DF24EFF-2928-44D4-AF70-C0F3DE6E083C}" name="Status"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -543,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC21A8D-7275-4F32-B667-4BF1F4B7FF51}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,7 +550,7 @@
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -567,204 +560,159 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="C15" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>